<commit_message>
opdater FEsv FEso og LnA
</commit_message>
<xml_diff>
--- a/data/original/Til Anders Peter og Frederik 14122023.xlsx
+++ b/data/original/Til Anders Peter og Frederik 14122023.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\ST_ENVS-Luft-Emi\Rikke\Sendt til div\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au277187_uni_au_dk/Documents/Documents/GitHub/AU-BCE-EE/Dalby-2024-KVIK/data/original/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_E6E2CDB5D714CECB874DAF8AF1372014E0ED704F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AED0E8BB-E1F2-4D74-BD4D-EC09953A6E8A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9765" windowHeight="9495"/>
+    <workbookView xWindow="225" yWindow="360" windowWidth="14955" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="N, TAN, TonGødning, VS" sheetId="1" r:id="rId1"/>
@@ -279,7 +280,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -373,25 +374,25 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Antal dyr" xfId="1"/>
-    <cellStyle name="Normal_N, TAN, TonGødning, VS" xfId="2"/>
+    <cellStyle name="Normal_Antal dyr" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal_N, TAN, TonGødning, VS" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -668,17 +669,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M324"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="A1:N1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B155" workbookViewId="0">
+      <selection activeCell="B171" sqref="A171:XFD171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="75.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
@@ -9912,7 +9913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:F135"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">

</xml_diff>